<commit_message>
fixed some package::function lacking and added species traits .
</commit_message>
<xml_diff>
--- a/1_data/1_data_nutrients/1_data_literature/1_data/0030_005_emerson_2007_bat/0030_005_emerson_2007.xlsx
+++ b/1_data/1_data_nutrients/1_data_literature/1_data/0030_005_emerson_2007_bat/0030_005_emerson_2007.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="109">
   <si>
     <t xml:space="preserve">reference_ID</t>
   </si>
@@ -639,15 +639,15 @@
   </sheetPr>
   <dimension ref="A1:CD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BL18" activeCellId="0" sqref="BL18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BI23" activeCellId="0" sqref="BI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.71"/>
@@ -658,23 +658,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="20.86"/>
@@ -689,7 +689,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="46" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="22.14"/>
@@ -699,15 +699,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="58" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="58" style="1" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="63" style="1" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="8.29"/>
@@ -715,7 +715,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="1" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="1" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="1" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="8.29"/>
@@ -2884,8 +2884,8 @@
       <c r="BF9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BG9" s="1" t="n">
-        <v>0.073</v>
+      <c r="BG9" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="BH9" s="1" t="s">
         <v>85</v>

</xml_diff>